<commit_message>
Update collection Excel template
</commit_message>
<xml_diff>
--- a/scripts/templates/cdisc_biomedical_concepts_latest_template.xlsx
+++ b/scripts/templates/cdisc_biomedical_concepts_latest_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\test\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\scripts\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7025333F-B13E-4CF9-B426-66AB6BFB64D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE05180-8C4B-4CE2-B89D-71308E554F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="915" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -80,13 +80,7 @@
     <t>bc_categories</t>
   </si>
   <si>
-    <t>Biomedical Concept category for the faciliation of API search and extract</t>
-  </si>
-  <si>
     <t>synonyms</t>
-  </si>
-  <si>
-    <t>Biomedical Concept synonym equivalent to BC short name for the facilitation of API search and extraction</t>
   </si>
   <si>
     <t>result_scales</t>
@@ -174,6 +168,12 @@
 There are currently {n} unique CDISC Biomedical Concepts in the CDISC Library.
 The image on the right shows the relation between Biomedical Concepts and SDTM Dataset Specializations.
 Only a few attributes are shown in the image.</t>
+  </si>
+  <si>
+    <t>Biomedical Concept categories for the faciliation of API search and extract</t>
+  </si>
+  <si>
+    <t>Biomedical Concept synonyms equivalent to BC short name for the facilitation of API search and extraction</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -650,100 +650,100 @@
         <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" ht="42.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="D15" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>9</v>
@@ -753,20 +753,20 @@
     <row r="18" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="13"/>
     </row>
@@ -796,7 +796,7 @@
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -834,37 +834,37 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="P1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +887,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -927,7 +927,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>14</v>
@@ -936,22 +936,22 @@
         <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>